<commit_message>
v2: Health Economics & Clinical Infrastructure Edition
Strip all sales/revenue data (NTS, TPS, business plans, competitive intel).
Rebuild as pure health economics tool with:
- Expanded stroke epidemiology (ischemic, LVO, MT eligible, hemorrhagic subtypes, AVM)
- Effective population calculation (age 65+ × 2.5 multiplier)
- Infrastructure score (0-100) replacing TPS
- Clinical priority tiers (Hub/Regional/Basic) replacing revenue tiers
- Infrastructure checklist (8 capabilities with ✓/✗)
- A-Fib epidemiology panel (conditional)
- Geographic access categories (Local/Short/Long/Flight)
- Updated analytics bar with clinical metrics
- Marker sizing by stroke volume instead of NTS

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample_hospitals.xlsx
+++ b/sample_hospitals.xlsx
@@ -27,14 +27,22 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000205B"/>
+        <bgColor rgb="0000205B"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -51,8 +59,8 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:AJ11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,30 +435,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="37" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="42" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="40" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="7" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
     <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
-    <col width="16" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="28" customWidth="1" min="12" max="12"/>
-    <col width="15" customWidth="1" min="13" max="13"/>
-    <col width="22" customWidth="1" min="14" max="14"/>
-    <col width="18" customWidth="1" min="15" max="15"/>
-    <col width="25" customWidth="1" min="16" max="16"/>
-    <col width="21" customWidth="1" min="17" max="17"/>
-    <col width="18" customWidth="1" min="18" max="18"/>
-    <col width="22" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="17" customWidth="1" min="21" max="21"/>
-    <col width="22" customWidth="1" min="22" max="22"/>
-    <col width="16" customWidth="1" min="23" max="23"/>
-    <col width="36" customWidth="1" min="24" max="24"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="14" customWidth="1" min="14" max="14"/>
+    <col width="16" customWidth="1" min="15" max="15"/>
+    <col width="18" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="16" customWidth="1" min="19" max="19"/>
+    <col width="14" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="12" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="12" customWidth="1" min="24" max="24"/>
+    <col width="14" customWidth="1" min="25" max="25"/>
+    <col width="10" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="10" customWidth="1" min="28" max="28"/>
+    <col width="12" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="14" customWidth="1" min="31" max="31"/>
+    <col width="10" customWidth="1" min="32" max="32"/>
+    <col width="14" customWidth="1" min="33" max="33"/>
+    <col width="12" customWidth="1" min="34" max="34"/>
+    <col width="10" customWidth="1" min="35" max="35"/>
+    <col width="40" customWidth="1" min="36" max="36"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -501,49 +521,49 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Licensed Beds</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Affiliation</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Buy Group/GPO</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Stroke Certification</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Strokes Per Year</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>IR Phone</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Licensed Beds</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Affiliation</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Buy Group/GPO</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Stroke Certification</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Cert Body</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Neurosurgery Fellowship</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Neuro IR Fellowship</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Strokes Per Year</t>
-        </is>
-      </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Catchment Population</t>
@@ -551,25 +571,85 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
+          <t>Population 65+</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>Median Age</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Life Expectancy</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>NTS 2025 (Full Year)</t>
-        </is>
-      </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>NTS 2026 (YTD)</t>
+          <t>CAH Status</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Telestroke Capable</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>24/7 Thrombectomy</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>tPA Available</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Neuro ICU</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>CT Scanner</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Spoke Hospital</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>A-Fib Prevalence</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>A-Fib Absolute Count</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>MMAE Score</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Clinical Benefit Radius (km)</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Medevac Available</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Road Access</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
@@ -583,7 +663,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Baptist Jacksonville</t>
+          <t>Baptist Jax</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -617,61 +697,97 @@
           <t>(904) 202-2000</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="n">
+        <v>972</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Baptist Health</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Vizient</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>900</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>(904) 202-2100</t>
         </is>
       </c>
-      <c r="K2" t="n">
-        <v>972</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Baptist Health</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Vizient</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>CSC</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Joint Commission</t>
         </is>
       </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
       <c r="Q2" t="b">
         <v>1</v>
       </c>
-      <c r="R2" t="n">
-        <v>900</v>
+      <c r="R2" t="b">
+        <v>1</v>
       </c>
       <c r="S2" t="n">
         <v>1750000</v>
       </c>
       <c r="T2" t="n">
+        <v>310000</v>
+      </c>
+      <c r="U2" t="n">
         <v>37.5</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>77.40000000000001</v>
       </c>
-      <c r="V2" t="n">
-        <v>26327</v>
-      </c>
-      <c r="W2" t="n">
-        <v>46025</v>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>175% YoY growth</t>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>56000</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>72</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>45</v>
+      </c>
+      <c r="AH2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Flagship CSC — 175% YoY growth in thrombectomy</t>
         </is>
       </c>
     </row>
@@ -707,71 +823,107 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>30.354</v>
+        <v>30.3554</v>
       </c>
       <c r="H3" t="n">
-        <v>-81.672</v>
+        <v>-81.6721</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>(904) 244-0411</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" t="n">
+        <v>695</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>University of Florida Health</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Vizient</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>750</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>(904) 244-0500</t>
         </is>
       </c>
-      <c r="K3" t="n">
-        <v>695</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>UF Health</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Vizient</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>CSC</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Joint Commission</t>
         </is>
       </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
       <c r="Q3" t="b">
         <v>1</v>
       </c>
-      <c r="R3" t="n">
-        <v>750</v>
+      <c r="R3" t="b">
+        <v>1</v>
       </c>
       <c r="S3" t="n">
         <v>1400000</v>
       </c>
       <c r="T3" t="n">
+        <v>238000</v>
+      </c>
+      <c r="U3" t="n">
         <v>36.8</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>76.90000000000001</v>
       </c>
-      <c r="V3" t="n">
-        <v>22150</v>
-      </c>
-      <c r="W3" t="n">
-        <v>18400</v>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Strong academic program</t>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>40600</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>68</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>40</v>
+      </c>
+      <c r="AH3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>Academic medical center with active NIR fellowship</t>
         </is>
       </c>
     </row>
@@ -783,7 +935,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mayo Clinic Jax</t>
+          <t>Mayo Jax</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -807,7 +959,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>30.2614</v>
+        <v>30.2617</v>
       </c>
       <c r="H4" t="n">
         <v>-81.4408</v>
@@ -817,283 +969,379 @@
           <t>(904) 953-2000</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" t="n">
+        <v>304</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Mayo Clinic Health System</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Mayo GPO</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>420</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>(904) 953-2100</t>
         </is>
       </c>
-      <c r="K4" t="n">
-        <v>304</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Mayo Clinic</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Mayo GPO</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>CSC</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>Joint Commission</t>
         </is>
       </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
       <c r="Q4" t="b">
         <v>1</v>
       </c>
-      <c r="R4" t="n">
-        <v>620</v>
+      <c r="R4" t="b">
+        <v>1</v>
       </c>
       <c r="S4" t="n">
-        <v>1200000</v>
+        <v>900000</v>
       </c>
       <c r="T4" t="n">
+        <v>171000</v>
+      </c>
+      <c r="U4" t="n">
         <v>42.1</v>
       </c>
-      <c r="U4" t="n">
-        <v>80.2</v>
-      </c>
       <c r="V4" t="n">
-        <v>19800</v>
-      </c>
-      <c r="W4" t="n">
-        <v>17500</v>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Premium facility</t>
+        <v>81.2</v>
+      </c>
+      <c r="W4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>34200</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>85</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AH4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>Research-intensive — leading DEFUSE trials enrollment</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Emory University Hospital</t>
+          <t>Ascension St. Vincent's Riverside</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Emory Atlanta</t>
+          <t>St. Vincent's</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1364 Clifton Rd NE, Atlanta, GA 30322</t>
+          <t>1 Shircliff Way, Jacksonville, FL 32204</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DeKalb County, GA</t>
+          <t>Duval County, FL</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>33.7942</v>
+        <v>30.3136</v>
       </c>
       <c r="H5" t="n">
-        <v>-84.32380000000001</v>
+        <v>-81.6892</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(404) 712-2000</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>(404) 712-2100</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>733</v>
+          <t>(904) 308-7300</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>528</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Ascension Health</t>
+        </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Emory Healthcare</t>
+          <t>HPG</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Vizient</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>CSC</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Joint Commission</t>
-        </is>
-      </c>
-      <c r="P5" t="b">
-        <v>1</v>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>340</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>DNV</t>
+        </is>
       </c>
       <c r="Q5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" t="n">
-        <v>1100</v>
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>2200000</v>
+        <v>850000</v>
       </c>
       <c r="T5" t="n">
-        <v>34.2</v>
+        <v>144500</v>
       </c>
       <c r="U5" t="n">
-        <v>76.5</v>
+        <v>39.2</v>
       </c>
       <c r="V5" t="n">
-        <v>31500</v>
-      </c>
-      <c r="W5" t="n">
-        <v>28000</v>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>Largest neuro program in territory</t>
+        <v>78.09999999999999</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>21250</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>55</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>Growing stroke program under new medical director</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Grady Memorial Hospital</t>
+          <t>Memorial Hospital Jacksonville</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Grady Atlanta</t>
+          <t>Memorial Jax</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>80 Jesse Hill Jr Dr SE, Atlanta, GA 30303</t>
+          <t>3625 University Blvd S, Jacksonville, FL 32216</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Fulton County, GA</t>
+          <t>Duval County, FL</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>33.7534</v>
+        <v>30.2843</v>
       </c>
       <c r="H6" t="n">
-        <v>-84.3845</v>
+        <v>-81.60209999999999</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(404) 616-1000</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>(404) 616-1100</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>953</v>
+          <t>(904) 702-6111</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>453</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Emory Healthcare</t>
+          <t>HealthTrust</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Premier</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>CSC</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>280</v>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
         <is>
           <t>Joint Commission</t>
         </is>
       </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
       <c r="Q6" t="b">
         <v>0</v>
       </c>
-      <c r="R6" t="n">
-        <v>950</v>
+      <c r="R6" t="b">
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>2500000</v>
+        <v>700000</v>
       </c>
       <c r="T6" t="n">
-        <v>33.8</v>
+        <v>119000</v>
       </c>
       <c r="U6" t="n">
-        <v>74.09999999999999</v>
+        <v>38.4</v>
       </c>
       <c r="V6" t="n">
-        <v>28700</v>
-      </c>
-      <c r="W6" t="n">
-        <v>25100</v>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>High volume trauma center</t>
-        </is>
-      </c>
+        <v>77.8</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>14700</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>48</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AH6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tallahassee Memorial HealthCare</t>
+          <t>Flagler Hospital</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TMH Tallahassee</t>
+          <t>Flagler</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1300 Miccosukee Rd, Tallahassee, FL 32308</t>
+          <t>400 Health Park Blvd, St. Augustine, FL 32086</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Augustine</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1103,93 +1351,129 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Leon County, FL</t>
+          <t>St. Johns County, FL</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>30.4558</v>
+        <v>29.8723</v>
       </c>
       <c r="H7" t="n">
-        <v>-84.253</v>
+        <v>-81.3168</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(850) 431-1155</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>772</v>
+          <t>(904) 819-5155</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>335</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Flagler Health+</t>
+        </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>TMH Healthcare</t>
+          <t>Premier</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>HealthTrust</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
           <t>PSC</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>DNV</t>
-        </is>
-      </c>
-      <c r="P7" t="b">
-        <v>0</v>
+      <c r="N7" t="n">
+        <v>210</v>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
       </c>
       <c r="Q7" t="b">
         <v>0</v>
       </c>
-      <c r="R7" t="n">
-        <v>420</v>
+      <c r="R7" t="b">
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>600000</v>
+        <v>350000</v>
       </c>
       <c r="T7" t="n">
-        <v>35.9</v>
+        <v>77000</v>
       </c>
       <c r="U7" t="n">
-        <v>77.8</v>
+        <v>44.6</v>
       </c>
       <c r="V7" t="n">
-        <v>12400</v>
-      </c>
-      <c r="W7" t="n">
-        <v>10800</v>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>Regional stroke center</t>
+        <v>79.5</v>
+      </c>
+      <c r="W7" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>10850</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>42</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>20</v>
+      </c>
+      <c r="AH7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>Spoke to Baptist Jax — telestroke hub model</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Orlando Regional Medical Center</t>
+          <t>Orange Park Medical Center</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ORMC Orlando</t>
+          <t>Orange Park</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>52 W Underwood St, Orlando, FL 32806</t>
+          <t>2001 Kingsley Ave, Orange Park, FL 32073</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orange Park</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1199,197 +1483,257 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Orange County, FL</t>
+          <t>Clay County, FL</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>28.5377</v>
+        <v>30.1665</v>
       </c>
       <c r="H8" t="n">
-        <v>-81.3783</v>
+        <v>-81.7178</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>(321) 841-5111</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>(321) 841-5200</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>808</v>
+          <t>(904) 639-8500</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>317</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Orlando Health</t>
+          <t>HealthTrust</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Vizient</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>CSC</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>Joint Commission</t>
-        </is>
-      </c>
-      <c r="P8" t="b">
-        <v>1</v>
+          <t>TSC</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>180</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>DNV</t>
+        </is>
       </c>
       <c r="Q8" t="b">
-        <v>1</v>
-      </c>
-      <c r="R8" t="n">
-        <v>850</v>
+        <v>0</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>1800000</v>
+        <v>280000</v>
       </c>
       <c r="T8" t="n">
-        <v>35.4</v>
+        <v>47600</v>
       </c>
       <c r="U8" t="n">
-        <v>78.09999999999999</v>
+        <v>36.9</v>
       </c>
       <c r="V8" t="n">
-        <v>24600</v>
-      </c>
-      <c r="W8" t="n">
-        <v>21800</v>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>Level 1 trauma center</t>
-        </is>
-      </c>
+        <v>77.2</v>
+      </c>
+      <c r="W8" t="b">
+        <v>0</v>
+      </c>
+      <c r="X8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>5040</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>35</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>15</v>
+      </c>
+      <c r="AH8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Memorial Regional Hospital</t>
+          <t>Southeast Georgia Health System - Brunswick</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Memorial Hollywood</t>
+          <t>SGHS Brunswick</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3501 Johnson St, Hollywood, FL 33021</t>
+          <t>2415 Parkwood Dr, Brunswick, GA 31520</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hollywood</t>
+          <t>Brunswick</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>FL</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Broward County, FL</t>
+          <t>Glynn County, GA</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>26.0216</v>
+        <v>31.1496</v>
       </c>
       <c r="H9" t="n">
-        <v>-80.1798</v>
+        <v>-81.4746</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>(954) 987-2000</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>(954) 987-2100</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>1042</v>
+          <t>(912) 466-7000</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>532</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Southeast Georgia Health System</t>
+        </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Memorial Healthcare System</t>
+          <t>Vizient</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Premier</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
           <t>PSC</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="N9" t="n">
+        <v>190</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
         <is>
           <t>Joint Commission</t>
         </is>
       </c>
-      <c r="P9" t="b">
-        <v>0</v>
-      </c>
       <c r="Q9" t="b">
-        <v>1</v>
-      </c>
-      <c r="R9" t="n">
-        <v>580</v>
+        <v>0</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>950000</v>
+        <v>320000</v>
       </c>
       <c r="T9" t="n">
-        <v>40.2</v>
+        <v>60800</v>
       </c>
       <c r="U9" t="n">
-        <v>78.8</v>
+        <v>40.3</v>
       </c>
       <c r="V9" t="n">
-        <v>15200</v>
-      </c>
-      <c r="W9" t="n">
-        <v>13100</v>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>Growing neuro program</t>
+        <v>75.8</v>
+      </c>
+      <c r="W9" t="b">
+        <v>0</v>
+      </c>
+      <c r="X9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>7680</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>25</v>
+      </c>
+      <c r="AH9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>Nearest CSC transfer is 90 min — medevac critical</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Augusta University Medical Center</t>
+          <t>Memorial Health University Medical Center</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AU Medical Augusta</t>
+          <t>Memorial Savannah</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1120 15th St, Augusta, GA 30912</t>
+          <t>4700 Waters Ave, Savannah, GA 31404</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Augusta</t>
+          <t>Savannah</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1399,97 +1743,133 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Richmond County, GA</t>
+          <t>Chatham County, GA</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>33.461</v>
+        <v>32.0312</v>
       </c>
       <c r="H10" t="n">
-        <v>-81.96899999999999</v>
+        <v>-81.0874</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>(706) 721-0211</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>(706) 721-0300</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>478</v>
+          <t>(912) 350-8000</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>612</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Augusta University Health</t>
+          <t>HealthTrust</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Vizient</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>PSC</t>
-        </is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>580</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
+          <t>(912) 350-8200</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
           <t>Joint Commission</t>
         </is>
       </c>
-      <c r="P10" t="b">
-        <v>1</v>
-      </c>
       <c r="Q10" t="b">
-        <v>0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>380</v>
+        <v>1</v>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>550000</v>
+        <v>680000</v>
       </c>
       <c r="T10" t="n">
-        <v>36.1</v>
+        <v>108800</v>
       </c>
       <c r="U10" t="n">
-        <v>75.59999999999999</v>
+        <v>35.7</v>
       </c>
       <c r="V10" t="n">
-        <v>8900</v>
-      </c>
-      <c r="W10" t="n">
-        <v>7200</v>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>Academic medical center</t>
+        <v>75.2</v>
+      </c>
+      <c r="W10" t="b">
+        <v>0</v>
+      </c>
+      <c r="X10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>18360</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>62</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>35</v>
+      </c>
+      <c r="AH10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>Regional CSC hub for southeast Georgia</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Flagler Hospital</t>
+          <t>Putnam Community Medical Center</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Flagler St Augustine</t>
+          <t>Putnam</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400 Health Park Blvd, St Augustine, FL 32086</t>
+          <t>611 Zeagler Dr, Palatka, FL 32177</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>St Augustine</t>
+          <t>Palatka</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1499,71 +1879,103 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>St Johns County, FL</t>
+          <t>Putnam County, FL</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>29.871</v>
+        <v>29.6516</v>
       </c>
       <c r="H11" t="n">
-        <v>-81.315</v>
+        <v>-81.6568</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>(904) 819-5155</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="n">
-        <v>335</v>
+          <t>(386) 328-5711</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>99</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>ScionHealth</t>
+        </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Flagler Health+</t>
+          <t>HealthTrust</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>HealthTrust</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>TSC</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>DNV</t>
-        </is>
-      </c>
-      <c r="P11" t="b">
-        <v>0</v>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>45</v>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="b">
         <v>0</v>
       </c>
-      <c r="R11" t="n">
-        <v>180</v>
+      <c r="R11" t="b">
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>280000</v>
+        <v>75000</v>
       </c>
       <c r="T11" t="n">
-        <v>45.3</v>
+        <v>15000</v>
       </c>
       <c r="U11" t="n">
-        <v>80.09999999999999</v>
+        <v>42.8</v>
       </c>
       <c r="V11" t="n">
-        <v>4200</v>
-      </c>
-      <c r="W11" t="n">
-        <v>3500</v>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>Smaller community hospital</t>
+        <v>73.59999999999999</v>
+      </c>
+      <c r="W11" t="b">
+        <v>1</v>
+      </c>
+      <c r="X11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>1125</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>18</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>Critical access — rural area, limited neurovascular capability</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add all 21 FL/GA territory hospitals
Full territory build with real facility data:
- 11 CSCs, 9 PSCs, 1 TSC across Florida and Georgia
- 13,493 total beds, 9,700 observed strokes/yr
- Est. 9,725 LVO cases, 6,807 MT eligible
- Avg infrastructure score: 74
- Includes Baptist Jax, UF Shands, Mayo, AdventHealth Orlando,
  TMH, Halifax Health, Memorial Savannah, St. Joseph's Tampa,
  and 13 more facilities

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample_hospitals.xlsx
+++ b/sample_hospitals.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ11"/>
+  <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,42 +435,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="42" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="45" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
-    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
     <col width="10" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="34" customWidth="1" min="11" max="11"/>
     <col width="14" customWidth="1" min="12" max="12"/>
     <col width="18" customWidth="1" min="13" max="13"/>
     <col width="14" customWidth="1" min="14" max="14"/>
-    <col width="16" customWidth="1" min="15" max="15"/>
-    <col width="18" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
-    <col width="12" customWidth="1" min="18" max="18"/>
-    <col width="16" customWidth="1" min="19" max="19"/>
-    <col width="14" customWidth="1" min="20" max="20"/>
-    <col width="10" customWidth="1" min="21" max="21"/>
-    <col width="12" customWidth="1" min="22" max="22"/>
-    <col width="10" customWidth="1" min="23" max="23"/>
-    <col width="12" customWidth="1" min="24" max="24"/>
-    <col width="14" customWidth="1" min="25" max="25"/>
-    <col width="10" customWidth="1" min="26" max="26"/>
-    <col width="10" customWidth="1" min="27" max="27"/>
-    <col width="10" customWidth="1" min="28" max="28"/>
-    <col width="12" customWidth="1" min="29" max="29"/>
-    <col width="12" customWidth="1" min="30" max="30"/>
-    <col width="14" customWidth="1" min="31" max="31"/>
-    <col width="10" customWidth="1" min="32" max="32"/>
-    <col width="14" customWidth="1" min="33" max="33"/>
-    <col width="12" customWidth="1" min="34" max="34"/>
-    <col width="10" customWidth="1" min="35" max="35"/>
-    <col width="40" customWidth="1" min="36" max="36"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -658,56 +636,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Baptist Medical Center Jacksonville</t>
+          <t>Savannah Health Services LLC (Memorial Health)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Baptist Jax</t>
+          <t>Memorial Savannah</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>800 Prudential Dr, Jacksonville, FL 32207</t>
+          <t>4700 Waters Ave, Savannah, GA 31404</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Savannah</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>FL</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Duval County, FL</t>
+          <t>Chatham County, GA</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>30.3187</v>
+        <v>32.0312</v>
       </c>
       <c r="H2" t="n">
-        <v>-81.6568</v>
+        <v>-81.0874</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(904) 202-2000</t>
+          <t>(912) 350-8000</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>972</v>
+        <v>612</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Baptist Health</t>
+          <t>HCA Healthcare</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Vizient</t>
+          <t>HealthTrust</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -716,11 +694,11 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>900</v>
+        <v>580</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>(904) 202-2100</t>
+          <t>(912) 350-8200</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -732,19 +710,19 @@
         <v>1</v>
       </c>
       <c r="R2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>1750000</v>
+        <v>680000</v>
       </c>
       <c r="T2" t="n">
-        <v>310000</v>
+        <v>108800</v>
       </c>
       <c r="U2" t="n">
-        <v>37.5</v>
+        <v>35.7</v>
       </c>
       <c r="V2" t="n">
-        <v>77.40000000000001</v>
+        <v>75.2</v>
       </c>
       <c r="W2" t="b">
         <v>0</v>
@@ -768,16 +746,16 @@
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="AE2" t="n">
-        <v>56000</v>
+        <v>18360</v>
       </c>
       <c r="AF2" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="AG2" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="AH2" t="b">
         <v>1</v>
@@ -787,29 +765,29 @@
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>Flagship CSC — 175% YoY growth in thrombectomy</t>
+          <t>Regional CSC hub for southeast Georgia</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UF Health Jacksonville</t>
+          <t>AdventHealth CSC</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UF Health Jax</t>
+          <t>AdventHealth CSC</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>655 W 8th St, Jacksonville, FL 32209</t>
+          <t>601 E Rollins St, Orlando, FL 32803</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Orlando</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -819,31 +797,31 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Duval County, FL</t>
+          <t>Orange County, FL</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>30.3554</v>
+        <v>28.5597</v>
       </c>
       <c r="H3" t="n">
-        <v>-81.6721</v>
+        <v>-81.36279999999999</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(904) 244-0411</t>
+          <t>(407) 303-5600</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>695</v>
+        <v>547</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>University of Florida Health</t>
+          <t>AdventHealth</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Vizient</t>
+          <t>Premier</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -852,11 +830,11 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>750</v>
+        <v>620</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>(904) 244-0500</t>
+          <t>(407) 303-5700</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -871,16 +849,16 @@
         <v>1</v>
       </c>
       <c r="S3" t="n">
-        <v>1400000</v>
+        <v>1200000</v>
       </c>
       <c r="T3" t="n">
-        <v>238000</v>
+        <v>192000</v>
       </c>
       <c r="U3" t="n">
-        <v>36.8</v>
+        <v>36.4</v>
       </c>
       <c r="V3" t="n">
-        <v>76.90000000000001</v>
+        <v>78.8</v>
       </c>
       <c r="W3" t="b">
         <v>0</v>
@@ -904,13 +882,13 @@
         <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="AE3" t="n">
-        <v>40600</v>
+        <v>36000</v>
       </c>
       <c r="AF3" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AG3" t="n">
         <v>40</v>
@@ -923,24 +901,24 @@
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>Academic medical center with active NIR fellowship</t>
+          <t>AdventHealth system CSC — strong neuro IR program</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mayo Clinic Jacksonville</t>
+          <t>Baptist Medical Center Jacksonville</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mayo Jax</t>
+          <t>Baptist Jax</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4500 San Pablo Rd S, Jacksonville, FL 32224</t>
+          <t>800 Prudential Dr, Jacksonville, FL 32207</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -959,27 +937,27 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>30.2617</v>
+        <v>30.3187</v>
       </c>
       <c r="H4" t="n">
-        <v>-81.4408</v>
+        <v>-81.6568</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(904) 953-2000</t>
+          <t>(904) 202-2000</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>304</v>
+        <v>972</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Mayo Clinic Health System</t>
+          <t>Baptist Health</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Mayo GPO</t>
+          <t>Vizient</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -988,11 +966,11 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>420</v>
+        <v>900</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>(904) 953-2100</t>
+          <t>(904) 202-2100</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -1007,16 +985,16 @@
         <v>1</v>
       </c>
       <c r="S4" t="n">
-        <v>900000</v>
+        <v>1750000</v>
       </c>
       <c r="T4" t="n">
-        <v>171000</v>
+        <v>310000</v>
       </c>
       <c r="U4" t="n">
-        <v>42.1</v>
+        <v>37.5</v>
       </c>
       <c r="V4" t="n">
-        <v>81.2</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="W4" t="b">
         <v>0</v>
@@ -1040,16 +1018,16 @@
         <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="AE4" t="n">
-        <v>34200</v>
+        <v>56000</v>
       </c>
       <c r="AF4" t="n">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="AG4" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AH4" t="b">
         <v>1</v>
@@ -1059,29 +1037,29 @@
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>Research-intensive — leading DEFUSE trials enrollment</t>
+          <t>Flagship CSC — largest stroke program in territory</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ascension St. Vincent's Riverside</t>
+          <t>Shands Teaching Hospital and Clinics (UF Health Shands)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>St. Vincent's</t>
+          <t>UF Shands GNV</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1 Shircliff Way, Jacksonville, FL 32204</t>
+          <t>1600 SW Archer Rd, Gainesville, FL 32610</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Gainesville</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1091,64 +1069,68 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Duval County, FL</t>
+          <t>Alachua County, FL</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>30.3136</v>
+        <v>29.64</v>
       </c>
       <c r="H5" t="n">
-        <v>-81.6892</v>
+        <v>-82.3443</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(904) 308-7300</t>
+          <t>(352) 265-0111</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>528</v>
+        <v>1162</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Ascension Health</t>
+          <t>University of Florida Health</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>HPG</t>
+          <t>Vizient</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>PSC</t>
+          <t>CSC</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>340</v>
-      </c>
-      <c r="O5" t="inlineStr"/>
+        <v>850</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>(352) 265-0200</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>DNV</t>
+          <t>Joint Commission</t>
         </is>
       </c>
       <c r="Q5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
-        <v>850000</v>
+        <v>950000</v>
       </c>
       <c r="T5" t="n">
-        <v>144500</v>
+        <v>152000</v>
       </c>
       <c r="U5" t="n">
-        <v>39.2</v>
+        <v>32.1</v>
       </c>
       <c r="V5" t="n">
-        <v>78.09999999999999</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="W5" t="b">
         <v>0</v>
@@ -1157,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="Y5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" t="b">
         <v>1</v>
@@ -1172,43 +1154,43 @@
         <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="AE5" t="n">
-        <v>21250</v>
+        <v>26600</v>
       </c>
       <c r="AF5" t="n">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="AG5" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AH5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" t="b">
         <v>1</v>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>Growing stroke program under new medical director</t>
+          <t>Academic flagship — full neurosurgery &amp; NIR fellowship programs</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Memorial Hospital Jacksonville</t>
+          <t>Shands Jacksonville Medical Center (UF Health Jax)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Memorial Jax</t>
+          <t>UF Health Jax</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3625 University Blvd S, Jacksonville, FL 32216</t>
+          <t>655 W 8th St, Jacksonville, FL 32209</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1227,60 +1209,64 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>30.2843</v>
+        <v>30.3554</v>
       </c>
       <c r="H6" t="n">
-        <v>-81.60209999999999</v>
+        <v>-81.6721</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(904) 702-6111</t>
+          <t>(904) 244-0411</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>453</v>
+        <v>695</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>HCA Healthcare</t>
+          <t>University of Florida Health</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>HealthTrust</t>
+          <t>Vizient</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>PSC</t>
+          <t>CSC</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>280</v>
-      </c>
-      <c r="O6" t="inlineStr"/>
+        <v>750</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>(904) 244-0500</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr">
         <is>
           <t>Joint Commission</t>
         </is>
       </c>
       <c r="Q6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="T6" t="n">
-        <v>119000</v>
+        <v>238000</v>
       </c>
       <c r="U6" t="n">
-        <v>38.4</v>
+        <v>36.8</v>
       </c>
       <c r="V6" t="n">
-        <v>77.8</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="W6" t="b">
         <v>0</v>
@@ -1289,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="Y6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" t="b">
         <v>1</v>
@@ -1304,44 +1290,48 @@
         <v>0</v>
       </c>
       <c r="AD6" t="n">
-        <v>2.1</v>
+        <v>2.9</v>
       </c>
       <c r="AE6" t="n">
-        <v>14700</v>
+        <v>40600</v>
       </c>
       <c r="AF6" t="n">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="AG6" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="AH6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" t="b">
         <v>1</v>
       </c>
-      <c r="AJ6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>Academic medical center with active NIR fellowship</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Flagler Hospital</t>
+          <t>Saint Joseph's Hospital</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Flagler</t>
+          <t>St. Joseph's Tampa</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>400 Health Park Blvd, St. Augustine, FL 32086</t>
+          <t>3001 W Dr Martin Luther King Jr Blvd, Tampa, FL 33607</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>St. Augustine</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1351,26 +1341,26 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>St. Johns County, FL</t>
+          <t>Hillsborough County, FL</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>29.8723</v>
+        <v>27.9632</v>
       </c>
       <c r="H7" t="n">
-        <v>-81.3168</v>
+        <v>-82.48739999999999</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(904) 819-5155</t>
+          <t>(813) 870-4000</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>335</v>
+        <v>897</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Flagler Health+</t>
+          <t>BayCare Health System</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1380,35 +1370,39 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>PSC</t>
+          <t>CSC</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>210</v>
-      </c>
-      <c r="O7" t="inlineStr"/>
+        <v>710</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>(813) 870-4100</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr">
         <is>
           <t>Joint Commission</t>
         </is>
       </c>
       <c r="Q7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" t="n">
-        <v>350000</v>
+        <v>1500000</v>
       </c>
       <c r="T7" t="n">
-        <v>77000</v>
+        <v>255000</v>
       </c>
       <c r="U7" t="n">
-        <v>44.6</v>
+        <v>36.2</v>
       </c>
       <c r="V7" t="n">
-        <v>79.5</v>
+        <v>78</v>
       </c>
       <c r="W7" t="b">
         <v>0</v>
@@ -1417,63 +1411,63 @@
         <v>1</v>
       </c>
       <c r="Y7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7" t="b">
         <v>1</v>
       </c>
       <c r="AA7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7" t="b">
         <v>1</v>
       </c>
       <c r="AC7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" t="n">
         <v>3.1</v>
       </c>
       <c r="AE7" t="n">
-        <v>10850</v>
+        <v>46500</v>
       </c>
       <c r="AF7" t="n">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="AG7" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="AH7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" t="b">
         <v>1</v>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>Spoke to Baptist Jax — telestroke hub model</t>
+          <t>Major Tampa Bay CSC — Pepin Heart &amp; Vascular Institute</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Orange Park Medical Center</t>
+          <t>Saint Vincent's Medical Center Riverside</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Orange Park</t>
+          <t>St. Vincent's Jax</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2001 Kingsley Ave, Orange Park, FL 32073</t>
+          <t>1 Shircliff Way, Jacksonville, FL 32204</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Orange Park</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1483,40 +1477,40 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Clay County, FL</t>
+          <t>Duval County, FL</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>30.1665</v>
+        <v>30.3136</v>
       </c>
       <c r="H8" t="n">
-        <v>-81.7178</v>
+        <v>-81.6892</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>(904) 639-8500</t>
+          <t>(904) 308-7300</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>317</v>
+        <v>528</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>HCA Healthcare</t>
+          <t>Ascension Health</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>HealthTrust</t>
+          <t>HPG</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>TSC</t>
+          <t>PSC</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>180</v>
+        <v>340</v>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
@@ -1531,16 +1525,16 @@
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>280000</v>
+        <v>850000</v>
       </c>
       <c r="T8" t="n">
-        <v>47600</v>
+        <v>144500</v>
       </c>
       <c r="U8" t="n">
-        <v>36.9</v>
+        <v>39.2</v>
       </c>
       <c r="V8" t="n">
-        <v>77.2</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="W8" t="b">
         <v>0</v>
@@ -1555,25 +1549,25 @@
         <v>1</v>
       </c>
       <c r="AA8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8" t="b">
         <v>1</v>
       </c>
       <c r="AC8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="AE8" t="n">
-        <v>5040</v>
+        <v>21250</v>
       </c>
       <c r="AF8" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="AG8" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AH8" t="b">
         <v>0</v>
@@ -1581,61 +1575,65 @@
       <c r="AI8" t="b">
         <v>1</v>
       </c>
-      <c r="AJ8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>Growing stroke program under new medical director</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Southeast Georgia Health System - Brunswick</t>
+          <t>North Florida Regional Medical Center</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SGHS Brunswick</t>
+          <t>N FL Regional</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2415 Parkwood Dr, Brunswick, GA 31520</t>
+          <t>6500 W Newberry Rd, Gainesville, FL 32605</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Brunswick</t>
+          <t>Gainesville</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Glynn County, GA</t>
+          <t>Alachua County, FL</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>31.1496</v>
+        <v>29.6661</v>
       </c>
       <c r="H9" t="n">
-        <v>-81.4746</v>
+        <v>-82.41459999999999</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>(912) 466-7000</t>
+          <t>(352) 333-4000</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>532</v>
+        <v>510</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Southeast Georgia Health System</t>
+          <t>HCA Healthcare</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Vizient</t>
+          <t>HealthTrust</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1644,7 +1642,7 @@
         </is>
       </c>
       <c r="N9" t="n">
-        <v>190</v>
+        <v>290</v>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
@@ -1659,16 +1657,16 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>320000</v>
+        <v>480000</v>
       </c>
       <c r="T9" t="n">
-        <v>60800</v>
+        <v>81600</v>
       </c>
       <c r="U9" t="n">
-        <v>40.3</v>
+        <v>34.5</v>
       </c>
       <c r="V9" t="n">
-        <v>75.8</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="W9" t="b">
         <v>0</v>
@@ -1692,82 +1690,82 @@
         <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="AE9" t="n">
-        <v>7680</v>
+        <v>10560</v>
       </c>
       <c r="AF9" t="n">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AG9" t="n">
         <v>25</v>
       </c>
       <c r="AH9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9" t="b">
         <v>1</v>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
-          <t>Nearest CSC transfer is 90 min — medevac critical</t>
+          <t>HCA facility — competes with UF Shands locally</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Memorial Health University Medical Center</t>
+          <t>Tallahassee Memorial HealthCare</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Memorial Savannah</t>
+          <t>TMH</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4700 Waters Ave, Savannah, GA 31404</t>
+          <t>1300 Miccosukee Rd, Tallahassee, FL 32308</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Savannah</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Chatham County, GA</t>
+          <t>Leon County, FL</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>32.0312</v>
+        <v>30.4408</v>
       </c>
       <c r="H10" t="n">
-        <v>-81.0874</v>
+        <v>-84.24299999999999</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>(912) 350-8000</t>
+          <t>(850) 431-1155</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>612</v>
+        <v>772</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>HCA Healthcare</t>
+          <t>Tallahassee Memorial HealthCare</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>HealthTrust</t>
+          <t>Premier</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1776,11 +1774,11 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>580</v>
+        <v>520</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>(912) 350-8200</t>
+          <t>(850) 431-1200</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1795,16 +1793,16 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>680000</v>
+        <v>550000</v>
       </c>
       <c r="T10" t="n">
-        <v>108800</v>
+        <v>82500</v>
       </c>
       <c r="U10" t="n">
-        <v>35.7</v>
+        <v>33.8</v>
       </c>
       <c r="V10" t="n">
-        <v>75.2</v>
+        <v>77.5</v>
       </c>
       <c r="W10" t="b">
         <v>0</v>
@@ -1828,13 +1826,13 @@
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
       <c r="AE10" t="n">
-        <v>18360</v>
+        <v>13200</v>
       </c>
       <c r="AF10" t="n">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AG10" t="n">
         <v>35</v>
@@ -1847,29 +1845,29 @@
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
-          <t>Regional CSC hub for southeast Georgia</t>
+          <t>Only CSC between Jacksonville and Pensacola</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Putnam Community Medical Center</t>
+          <t>Shands Teaching Hospital (UF Health Rehab)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Putnam</t>
+          <t>UF Shands Rehab</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>611 Zeagler Dr, Palatka, FL 32177</t>
+          <t>101 Newell Dr, Gainesville, FL 32611</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Palatka</t>
+          <t>Gainesville</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1879,103 +1877,1563 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Putnam County, FL</t>
+          <t>Alachua County, FL</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>29.6516</v>
+        <v>29.641</v>
       </c>
       <c r="H11" t="n">
-        <v>-81.6568</v>
+        <v>-82.3468</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>(386) 328-5711</t>
+          <t>(352) 265-0500</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>99</v>
+        <v>240</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>ScionHealth</t>
+          <t>University of Florida Health</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
+          <t>Vizient</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>180</v>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>450000</v>
+      </c>
+      <c r="T11" t="n">
+        <v>72000</v>
+      </c>
+      <c r="U11" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="V11" t="n">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="W11" t="b">
+        <v>0</v>
+      </c>
+      <c r="X11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>9000</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>38</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>20</v>
+      </c>
+      <c r="AH11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>Satellite campus of UF Health — spoke to main Shands CSC</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HCA Lake Monroe (Central Florida Regional)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>HCA Lake Monroe</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1401 W Seminole Blvd, Sanford, FL 32771</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sanford</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Seminole County, FL</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>28.812</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-81.2804</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>(407) 321-4500</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>226</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
           <t>HealthTrust</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="N11" t="n">
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>160</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>350000</v>
+      </c>
+      <c r="T12" t="n">
+        <v>63000</v>
+      </c>
+      <c r="U12" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="V12" t="n">
+        <v>78.2</v>
+      </c>
+      <c r="W12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>8050</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>35</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>15</v>
+      </c>
+      <c r="AH12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HCA Florida Lawnwood Hospital</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>HCA Lawnwood</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1700 S 23rd St, Fort Pierce, FL 34950</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Fort Pierce</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>St. Lucie County, FL</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>27.4355</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-80.34529999999999</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>(772) 461-4000</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>380</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>HealthTrust</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>250</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>420000</v>
+      </c>
+      <c r="T13" t="n">
+        <v>88200</v>
+      </c>
+      <c r="U13" t="n">
+        <v>42.7</v>
+      </c>
+      <c r="V13" t="n">
+        <v>77</v>
+      </c>
+      <c r="W13" t="b">
+        <v>0</v>
+      </c>
+      <c r="X13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>10920</v>
+      </c>
+      <c r="AF13" t="n">
         <v>45</v>
       </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>75000</v>
-      </c>
-      <c r="T11" t="n">
-        <v>15000</v>
-      </c>
-      <c r="U11" t="n">
-        <v>42.8</v>
-      </c>
-      <c r="V11" t="n">
-        <v>73.59999999999999</v>
-      </c>
-      <c r="W11" t="b">
-        <v>1</v>
-      </c>
-      <c r="X11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>1125</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>18</v>
-      </c>
-      <c r="AG11" t="n">
-        <v>10</v>
-      </c>
-      <c r="AH11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AJ11" t="inlineStr">
-        <is>
-          <t>Critical access — rural area, limited neurovascular capability</t>
+      <c r="AG13" t="n">
+        <v>25</v>
+      </c>
+      <c r="AH13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>Treasure Coast stroke center — high 65+ population</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Bay Medical Sacred Heart Health System</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bay Medical PC</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>615 N Bonita Ave, Panama City, FL 32401</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Panama City</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Bay County, FL</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>30.1697</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-85.6636</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>(850) 769-1511</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>323</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Ascension/Sacred Heart</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>HPG</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>190</v>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>DNV</t>
+        </is>
+      </c>
+      <c r="Q14" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>280000</v>
+      </c>
+      <c r="T14" t="n">
+        <v>47600</v>
+      </c>
+      <c r="U14" t="n">
+        <v>39.8</v>
+      </c>
+      <c r="V14" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="W14" t="b">
+        <v>0</v>
+      </c>
+      <c r="X14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>5320</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>38</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>20</v>
+      </c>
+      <c r="AH14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>Panhandle region — nearest CSC is TMH (100+ mi)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mayo Clinic Jacksonville</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mayo Jax</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4500 San Pablo Rd S, Jacksonville, FL 32224</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Duval County, FL</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>30.2617</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-81.4408</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>(904) 953-2000</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>304</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Mayo Clinic Health System</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Mayo GPO</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>420</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>(904) 953-2100</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q15" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
+      <c r="S15" t="n">
+        <v>900000</v>
+      </c>
+      <c r="T15" t="n">
+        <v>171000</v>
+      </c>
+      <c r="U15" t="n">
+        <v>42.1</v>
+      </c>
+      <c r="V15" t="n">
+        <v>81.2</v>
+      </c>
+      <c r="W15" t="b">
+        <v>0</v>
+      </c>
+      <c r="X15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>34200</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>85</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>50</v>
+      </c>
+      <c r="AH15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>Research-intensive — leading clinical trials enrollment</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UF Health Heart &amp; Vascular and Neuromedicine Hospitals</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>UF Neuro Hospital</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1505 SW Archer Rd, Gainesville, FL 32608</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Gainesville</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Alachua County, FL</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>29.6375</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-82.34999999999999</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>(352) 265-8000</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>216</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>University of Florida Health</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Vizient</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>480</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>(352) 265-8100</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>600000</v>
+      </c>
+      <c r="T16" t="n">
+        <v>96000</v>
+      </c>
+      <c r="U16" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="V16" t="n">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="W16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>15600</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>80</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>40</v>
+      </c>
+      <c r="AH16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>New dedicated neurovascular hospital — state-of-the-art hybrid ORs</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Candler General Hospital</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Candler Savannah</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>5353 Reynolds St, Savannah, GA 31405</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Savannah</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Chatham County, GA</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>32.0098</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-81.11790000000001</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>(912) 819-6000</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>384</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>St. Joseph's/Candler Health System</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Premier</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>220</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q17" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>380000</v>
+      </c>
+      <c r="T17" t="n">
+        <v>64600</v>
+      </c>
+      <c r="U17" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="V17" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="W17" t="b">
+        <v>0</v>
+      </c>
+      <c r="X17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>8740</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>42</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>20</v>
+      </c>
+      <c r="AH17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>Part of St. Joseph's/Candler system in Savannah</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Malcom Randall VA Medical Center</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>VA Gainesville</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1601 SW Archer Rd, Gainesville, FL 32608</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Gainesville</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Alachua County, FL</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>29.6395</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-82.3455</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>(352) 376-1611</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>421</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>US Dept of Veterans Affairs</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>VA FSS</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>310</v>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>620000</v>
+      </c>
+      <c r="T18" t="n">
+        <v>167400</v>
+      </c>
+      <c r="U18" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="V18" t="n">
+        <v>74.8</v>
+      </c>
+      <c r="W18" t="b">
+        <v>0</v>
+      </c>
+      <c r="X18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>26040</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>52</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>VA facility — very high 65+ population, transfers complex cases to UF Shands</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Halifax Hospital Medical Center (Halifax Health)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Halifax Health</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>303 N Clyde Morris Blvd, Daytona Beach, FL 32114</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Daytona Beach</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Volusia County, FL</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>29.2184</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-81.0484</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>(386) 254-4000</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>678</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Halifax Health</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Vizient</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>490</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>(386) 254-4100</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q19" t="b">
+        <v>1</v>
+      </c>
+      <c r="R19" t="b">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>580000</v>
+      </c>
+      <c r="T19" t="n">
+        <v>110200</v>
+      </c>
+      <c r="U19" t="n">
+        <v>43.6</v>
+      </c>
+      <c r="V19" t="n">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="W19" t="b">
+        <v>0</v>
+      </c>
+      <c r="X19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>17400</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>60</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>35</v>
+      </c>
+      <c r="AH19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>Central FL east coast CSC — high retiree catchment</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Memorial Hospital Jacksonville</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Memorial Jax</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3625 University Blvd S, Jacksonville, FL 32216</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Duval County, FL</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>30.2843</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-81.60209999999999</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>(904) 702-6111</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>453</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>HealthTrust</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>280</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" t="b">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>700000</v>
+      </c>
+      <c r="T20" t="n">
+        <v>119000</v>
+      </c>
+      <c r="U20" t="n">
+        <v>38.4</v>
+      </c>
+      <c r="V20" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="W20" t="b">
+        <v>0</v>
+      </c>
+      <c r="X20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>14700</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>48</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>25</v>
+      </c>
+      <c r="AH20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Orange Park Medical Center</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Orange Park</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2001 Kingsley Ave, Orange Park, FL 32073</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Orange Park</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Clay County, FL</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>30.1665</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-81.7178</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>(904) 639-8500</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>317</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>HealthTrust</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>TSC</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>180</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>DNV</t>
+        </is>
+      </c>
+      <c r="Q21" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" t="b">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>280000</v>
+      </c>
+      <c r="T21" t="n">
+        <v>47600</v>
+      </c>
+      <c r="U21" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="V21" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="W21" t="b">
+        <v>0</v>
+      </c>
+      <c r="X21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>5040</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>35</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>15</v>
+      </c>
+      <c r="AH21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>AdventHealth Orlando</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AdventHealth ORL</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>601 E Rollins St, Orlando, FL 32803</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Orange County, FL</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>28.5727</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-81.3627</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>(407) 303-5600</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>2856</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>AdventHealth</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Premier</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>CSC</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>980</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>(407) 303-5800</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Joint Commission</t>
+        </is>
+      </c>
+      <c r="Q22" t="b">
+        <v>1</v>
+      </c>
+      <c r="R22" t="b">
+        <v>1</v>
+      </c>
+      <c r="S22" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="T22" t="n">
+        <v>336000</v>
+      </c>
+      <c r="U22" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="V22" t="n">
+        <v>79.09999999999999</v>
+      </c>
+      <c r="W22" t="b">
+        <v>0</v>
+      </c>
+      <c r="X22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>71400</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>82</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>50</v>
+      </c>
+      <c r="AH22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ22" t="inlineStr">
+        <is>
+          <t>Largest hospital in territory — 2,856 beds, massive catchment</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add GLP-1 RA usage data and collapsible sources panel
- Added 3 GLP-1 fields (Rx Rate, Market Penetration, Est Users) to all 21 hospitals
- GLP-1 section in drawer with purple-themed cards showing Rx/1k, penetration %, est users
- Clinical relevance note: SUSTAIN-6, LEADER, SELECT trial references
- Sources panel now collapsible with toggle arrow (starts collapsed)
- Added source [11] for GLP-1 data (CMS Part D / IQVIA / SELECT)
</commit_message>
<xml_diff>
--- a/sample_hospitals.xlsx
+++ b/sample_hospitals.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ22"/>
+  <dimension ref="A1:AM22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +629,21 @@
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
+          <t>GLP-1 Rx Rate</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>GLP-1 Market Penetration</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>GLP-1 Est Users</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
           <t>Comment</t>
         </is>
       </c>
@@ -763,7 +778,16 @@
       <c r="AI2" t="b">
         <v>1</v>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AJ2" t="n">
+        <v>58.4</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>14960</v>
+      </c>
+      <c r="AM2" t="inlineStr">
         <is>
           <t>Regional CSC hub — only Level I trauma in SE Georgia</t>
         </is>
@@ -899,7 +923,16 @@
       <c r="AI3" t="b">
         <v>1</v>
       </c>
-      <c r="AJ3" t="inlineStr">
+      <c r="AJ3" t="n">
+        <v>72.59999999999999</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>22780</v>
+      </c>
+      <c r="AM3" t="inlineStr">
         <is>
           <t>AdventHealth system CSC campus — DNV certified 2019</t>
         </is>
@@ -1035,7 +1068,16 @@
       <c r="AI4" t="b">
         <v>1</v>
       </c>
-      <c r="AJ4" t="inlineStr">
+      <c r="AJ4" t="n">
+        <v>64.2</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>42350</v>
+      </c>
+      <c r="AM4" t="inlineStr">
         <is>
           <t>Flagship CSC — largest stroke program in NE Florida</t>
         </is>
@@ -1171,7 +1213,16 @@
       <c r="AI5" t="b">
         <v>1</v>
       </c>
-      <c r="AJ5" t="inlineStr">
+      <c r="AJ5" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>18620</v>
+      </c>
+      <c r="AM5" t="inlineStr">
         <is>
           <t>Academic flagship — 1,043 stroke cases in 2024 (AHA data)</t>
         </is>
@@ -1307,7 +1358,16 @@
       <c r="AI6" t="b">
         <v>1</v>
       </c>
-      <c r="AJ6" t="inlineStr">
+      <c r="AJ6" t="n">
+        <v>62.1</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>33880</v>
+      </c>
+      <c r="AM6" t="inlineStr">
         <is>
           <t>Academic med center — TraumaOne helicopter stroke transport</t>
         </is>
@@ -1443,7 +1503,16 @@
       <c r="AI7" t="b">
         <v>1</v>
       </c>
-      <c r="AJ7" t="inlineStr">
+      <c r="AJ7" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>25.6</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>38250</v>
+      </c>
+      <c r="AM7" t="inlineStr">
         <is>
           <t>Pepin Heart &amp; Vascular Institute — BayCare system</t>
         </is>
@@ -1575,7 +1644,16 @@
       <c r="AI8" t="b">
         <v>1</v>
       </c>
-      <c r="AJ8" t="inlineStr">
+      <c r="AJ8" t="n">
+        <v>61.8</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>19640</v>
+      </c>
+      <c r="AM8" t="inlineStr">
         <is>
           <t>Ranked #3 in Jacksonville by U.S. News 2025</t>
         </is>
@@ -1707,7 +1785,16 @@
       <c r="AI9" t="b">
         <v>1</v>
       </c>
-      <c r="AJ9" t="inlineStr">
+      <c r="AJ9" t="n">
+        <v>54.3</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>10080</v>
+      </c>
+      <c r="AM9" t="inlineStr">
         <is>
           <t>HCA facility — CSC certified, serves 14 surrounding counties</t>
         </is>
@@ -1843,7 +1930,16 @@
       <c r="AI10" t="b">
         <v>1</v>
       </c>
-      <c r="AJ10" t="inlineStr">
+      <c r="AJ10" t="n">
+        <v>49.6</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>10560</v>
+      </c>
+      <c r="AM10" t="inlineStr">
         <is>
           <t>Only CSC between Jacksonville and Pensacola — serves 21 counties</t>
         </is>
@@ -1975,7 +2071,16 @@
       <c r="AI11" t="b">
         <v>1</v>
       </c>
-      <c r="AJ11" t="inlineStr">
+      <c r="AJ11" t="n">
+        <v>52.1</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>9130</v>
+      </c>
+      <c r="AM11" t="inlineStr">
         <is>
           <t>Satellite of UF Health — spoke to main Shands CSC</t>
         </is>
@@ -2107,7 +2212,16 @@
       <c r="AI12" t="b">
         <v>1</v>
       </c>
-      <c r="AJ12" t="inlineStr">
+      <c r="AJ12" t="n">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>25.1</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>8820</v>
+      </c>
+      <c r="AM12" t="inlineStr">
         <is>
           <t>Award-winning cardiac and stroke programs — CSC certified</t>
         </is>
@@ -2239,7 +2353,16 @@
       <c r="AI13" t="b">
         <v>1</v>
       </c>
-      <c r="AJ13" t="inlineStr">
+      <c r="AJ13" t="n">
+        <v>74.8</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>10920</v>
+      </c>
+      <c r="AM13" t="inlineStr">
         <is>
           <t>Treasure Coast — only Advanced Thrombectomy Center in St. Lucie County</t>
         </is>
@@ -2371,7 +2494,16 @@
       <c r="AI14" t="b">
         <v>1</v>
       </c>
-      <c r="AJ14" t="inlineStr">
+      <c r="AJ14" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>5150</v>
+      </c>
+      <c r="AM14" t="inlineStr">
         <is>
           <t>Panhandle Level II Trauma — nearest CSC is TMH (100+ mi)</t>
         </is>
@@ -2507,7 +2639,16 @@
       <c r="AI15" t="b">
         <v>1</v>
       </c>
-      <c r="AJ15" t="inlineStr">
+      <c r="AJ15" t="n">
+        <v>71.3</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>22140</v>
+      </c>
+      <c r="AM15" t="inlineStr">
         <is>
           <t>Ranked #1 in FL by U.S. News 2025 — expanded to 419 beds (2024)</t>
         </is>
@@ -2643,7 +2784,16 @@
       <c r="AI16" t="b">
         <v>1</v>
       </c>
-      <c r="AJ16" t="inlineStr">
+      <c r="AJ16" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>12540</v>
+      </c>
+      <c r="AM16" t="inlineStr">
         <is>
           <t>Opened 2017 — 7 neuro ORs incl. 2 intraoperative MRI suites</t>
         </is>
@@ -2775,7 +2925,16 @@
       <c r="AI17" t="b">
         <v>1</v>
       </c>
-      <c r="AJ17" t="inlineStr">
+      <c r="AJ17" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>21.8</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>8550</v>
+      </c>
+      <c r="AM17" t="inlineStr">
         <is>
           <t>Second-oldest US hospital in continuous operation (est. 1804)</t>
         </is>
@@ -2907,7 +3066,16 @@
       <c r="AI18" t="b">
         <v>1</v>
       </c>
-      <c r="AJ18" t="inlineStr">
+      <c r="AJ18" t="n">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>26040</v>
+      </c>
+      <c r="AM18" t="inlineStr">
         <is>
           <t>VA 1a High Complexity — very high 65+ population</t>
         </is>
@@ -3043,7 +3211,16 @@
       <c r="AI19" t="b">
         <v>1</v>
       </c>
-      <c r="AJ19" t="inlineStr">
+      <c r="AJ19" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>17400</v>
+      </c>
+      <c r="AM19" t="inlineStr">
         <is>
           <t>Thrombectomy-Capable cert renewed April 2025 — Level II Trauma</t>
         </is>
@@ -3175,7 +3352,16 @@
       <c r="AI20" t="b">
         <v>1</v>
       </c>
-      <c r="AJ20" t="inlineStr">
+      <c r="AJ20" t="n">
+        <v>60.5</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>16100</v>
+      </c>
+      <c r="AM20" t="inlineStr">
         <is>
           <t>America's 250 Best Hospitals Award (Healthgrades)</t>
         </is>
@@ -3307,7 +3493,16 @@
       <c r="AI21" t="b">
         <v>1</v>
       </c>
-      <c r="AJ21" t="inlineStr">
+      <c r="AJ21" t="n">
+        <v>57.3</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>5880</v>
+      </c>
+      <c r="AM21" t="inlineStr">
         <is>
           <t>Only Primary Stroke Center in Clay County — 6-county catchment</t>
         </is>
@@ -3443,7 +3638,16 @@
       <c r="AI22" t="b">
         <v>1</v>
       </c>
-      <c r="AJ22" t="inlineStr">
+      <c r="AJ22" t="n">
+        <v>69.8</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>25.9</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>54180</v>
+      </c>
+      <c r="AM22" t="inlineStr">
         <is>
           <t>3rd largest US hospital — $660M expansion adding 440 beds (2025)</t>
         </is>

</xml_diff>